<commit_message>
fixed error with invalid protocol names causing exception, created NB project
</commit_message>
<xml_diff>
--- a/examples/EMTF_vu13p/src/link_map_MPCX_CPPF_GE11.xlsx
+++ b/examples/EMTF_vu13p/src/link_map_MPCX_CPPF_GE11.xlsx
@@ -70,7 +70,7 @@
     <t xml:space="preserve">0</t>
   </si>
   <si>
-    <t xml:space="preserve">MPCX</t>
+    <t xml:space="preserve">mpcx</t>
   </si>
   <si>
     <t xml:space="preserve">C</t>
@@ -211,7 +211,7 @@
     <t xml:space="preserve">40</t>
   </si>
   <si>
-    <t xml:space="preserve">CPPF</t>
+    <t xml:space="preserve">cppf</t>
   </si>
   <si>
     <t xml:space="preserve">Q</t>
@@ -274,7 +274,7 @@
     <t xml:space="preserve">56</t>
   </si>
   <si>
-    <t xml:space="preserve">GE11</t>
+    <t xml:space="preserve">ge11</t>
   </si>
   <si>
     <t xml:space="preserve">ge11_rx</t>
@@ -584,8 +584,8 @@
   </sheetPr>
   <dimension ref="A1:H86"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K66" activeCellId="0" sqref="K66"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5:D67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>